<commit_message>
Fixed reservas & token
Fixed create & update reserva & token expiration logout
</commit_message>
<xml_diff>
--- a/utilizadoresBulk.xlsx
+++ b/utilizadoresBulk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f945419a16710a90/Documentos/GitHub/Pint21-22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{C0EBECC5-E325-4124-88B0-184EDCDD2C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED160851-A3D3-4E75-8ECC-BA5A377D6937}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{C0EBECC5-E325-4124-88B0-184EDCDD2C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A297240C-24AB-4568-A8F3-496F5F79D0CA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D91CBB16-FF8E-4C6C-92D7-CB864C65AB5A}"/>
   </bookViews>
@@ -53,100 +53,100 @@
     <t>Data Nascimento</t>
   </si>
   <si>
-    <t>bulkuser1</t>
-  </si>
-  <si>
-    <t>bulkuser2</t>
-  </si>
-  <si>
-    <t>bulkuser3</t>
-  </si>
-  <si>
-    <t>bulkuser4</t>
-  </si>
-  <si>
-    <t>bulkuser5</t>
-  </si>
-  <si>
-    <t>bulkuser6</t>
-  </si>
-  <si>
-    <t>bulkuser7</t>
-  </si>
-  <si>
-    <t>bulkuser8</t>
-  </si>
-  <si>
-    <t>bulkuser9</t>
-  </si>
-  <si>
-    <t>bulkuser10</t>
-  </si>
-  <si>
-    <t>Bulk User 1</t>
-  </si>
-  <si>
-    <t>Bulk User 2</t>
-  </si>
-  <si>
-    <t>Bulk User 3</t>
-  </si>
-  <si>
-    <t>Bulk User 4</t>
-  </si>
-  <si>
-    <t>Bulk User 5</t>
-  </si>
-  <si>
-    <t>Bulk User 6</t>
-  </si>
-  <si>
-    <t>Bulk User 7</t>
-  </si>
-  <si>
-    <t>Bulk User 8</t>
-  </si>
-  <si>
-    <t>Bulk User 9</t>
-  </si>
-  <si>
-    <t>Bulk User 10</t>
-  </si>
-  <si>
-    <t>bulkuser1@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser2@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser3@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser4@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser5@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser6@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser7@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser8@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser9@gmail.com</t>
-  </si>
-  <si>
-    <t>bulkuser10@gmail.com</t>
-  </si>
-  <si>
     <t>Passw0rd</t>
   </si>
   <si>
     <t>Tipo Utilizador</t>
+  </si>
+  <si>
+    <t>Bulk User 31</t>
+  </si>
+  <si>
+    <t>Bulk User 51</t>
+  </si>
+  <si>
+    <t>Bulk User 91</t>
+  </si>
+  <si>
+    <t>Bulk User 71</t>
+  </si>
+  <si>
+    <t>Bulk User 22</t>
+  </si>
+  <si>
+    <t>Bulk User 42</t>
+  </si>
+  <si>
+    <t>Bulk User 62</t>
+  </si>
+  <si>
+    <t>Bulk User 82</t>
+  </si>
+  <si>
+    <t>Bulk User 102</t>
+  </si>
+  <si>
+    <t>Bulk User 12</t>
+  </si>
+  <si>
+    <t>testebulkuser1</t>
+  </si>
+  <si>
+    <t>testebulkuser2</t>
+  </si>
+  <si>
+    <t>testebulkuser3</t>
+  </si>
+  <si>
+    <t>testebulkuser4</t>
+  </si>
+  <si>
+    <t>testebulkuser5</t>
+  </si>
+  <si>
+    <t>testebulkuser6</t>
+  </si>
+  <si>
+    <t>testebulkuser7</t>
+  </si>
+  <si>
+    <t>testebulkuser8</t>
+  </si>
+  <si>
+    <t>testebulkuser9</t>
+  </si>
+  <si>
+    <t>testebulkuser10</t>
+  </si>
+  <si>
+    <t>testebulkuser1@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser2@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser3@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser4@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser5@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser6@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser7@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser8@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser9@gmail.com</t>
+  </si>
+  <si>
+    <t>testebulkuser10@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,21 +549,21 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2">
         <v>35935</v>
@@ -574,16 +574,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2">
         <v>35936</v>
@@ -594,16 +594,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2">
         <v>35937</v>
@@ -614,16 +614,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2">
         <v>35938</v>
@@ -634,16 +634,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2">
         <v>35939</v>
@@ -654,16 +654,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2">
         <v>35940</v>
@@ -674,16 +674,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E8" s="2">
         <v>35941</v>
@@ -694,16 +694,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E9" s="2">
         <v>35942</v>
@@ -714,16 +714,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2">
         <v>35943</v>
@@ -734,16 +734,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2">
         <v>35944</v>

</xml_diff>